<commit_message>
added the realtime clock
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37457" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38207" uniqueCount="448">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1486,6 +1486,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId238</t>
   </si>
 </sst>
 </file>
@@ -5054,7 +5057,23 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="4:4"/>
+    <row r="125" spans="4:4">
+      <c r="B125" t="s">
+        <v>447</v>
+      </c>
+      <c r="C125" t="s">
+        <v>40</v>
+      </c>
+      <c r="D125" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125" t="s">
+        <v>46</v>
+      </c>
+      <c r="F125" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="126" spans="4:4"/>
     <row r="127" spans="4:4"/>
     <row r="128" spans="4:4"/>

</xml_diff>

<commit_message>
added bugs and events
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38207" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37484" uniqueCount="463">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1398,66 +1398,75 @@
     <t xml:space="preserve">SingleUseId208</t>
   </si>
   <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mriamc.ttf</t>
+  </si>
+  <si>
     <t xml:space="preserve">SingleUseId209</t>
   </si>
   <si>
-    <t xml:space="preserve">SingleUseId210</t>
+    <t xml:space="preserve">SingleUseId211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">вс</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId227</t>
   </si>
   <si>
     <t xml:space="preserve">08</t>
   </si>
   <si>
-    <t xml:space="preserve">SingleUseId211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId218</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId219</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId227</t>
-  </si>
-  <si>
     <t xml:space="preserve">SingleUseId228</t>
   </si>
   <si>
@@ -1489,6 +1498,42 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00-0xFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId248</t>
   </si>
 </sst>
 </file>
@@ -2832,7 +2877,9 @@
       </c>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="H7"/>
+      <c r="H7" t="s">
+        <v>457</v>
+      </c>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7" s="8" t="s">
@@ -2868,7 +2915,9 @@
         <v>25</v>
       </c>
       <c r="G8"/>
-      <c r="H8"/>
+      <c r="H8" t="s">
+        <v>457</v>
+      </c>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8" s="8" t="s">
@@ -2886,6 +2935,27 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C9" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" t="s">
+        <v>94</v>
+      </c>
       <c r="K9" s="12" t="s">
         <v>14</v>
       </c>
@@ -2903,6 +2973,27 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>457</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="12" t="s">
         <v>36</v>
       </c>
@@ -3045,7 +3136,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>419</v>
+        <v>380</v>
       </c>
       <c r="F6" t="s">
         <v>58</v>
@@ -3181,7 +3272,7 @@
         <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>419</v>
+        <v>380</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -3393,16 +3484,16 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="F27" t="s">
         <v>58</v>
@@ -3410,7 +3501,7 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="C28" t="s">
         <v>95</v>
@@ -3427,16 +3518,16 @@
     </row>
     <row r="29" spans="4:4">
       <c r="B29" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>380</v>
       </c>
       <c r="F29" t="s">
         <v>58</v>
@@ -3444,16 +3535,16 @@
     </row>
     <row r="30" spans="4:4">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
         <v>58</v>
@@ -3461,16 +3552,16 @@
     </row>
     <row r="31" spans="4:4">
       <c r="B31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>380</v>
+        <v>92</v>
       </c>
       <c r="F31" t="s">
         <v>58</v>
@@ -3478,16 +3569,16 @@
     </row>
     <row r="32" spans="4:4">
       <c r="B32" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>381</v>
       </c>
       <c r="F32" t="s">
         <v>58</v>
@@ -3495,16 +3586,16 @@
     </row>
     <row r="33" spans="4:4">
       <c r="B33" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -3512,16 +3603,16 @@
     </row>
     <row r="34" spans="4:4">
       <c r="B34" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>381</v>
+        <v>175</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -3529,16 +3620,16 @@
     </row>
     <row r="35" spans="4:4">
       <c r="B35" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F35" t="s">
         <v>58</v>
@@ -3546,16 +3637,16 @@
     </row>
     <row r="36" spans="4:4">
       <c r="B36" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="F36" t="s">
         <v>58</v>
@@ -3563,16 +3654,16 @@
     </row>
     <row r="37" spans="4:4">
       <c r="B37" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C37" t="s">
         <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -3580,16 +3671,16 @@
     </row>
     <row r="38" spans="4:4">
       <c r="B38" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F38" t="s">
         <v>58</v>
@@ -3597,16 +3688,16 @@
     </row>
     <row r="39" spans="4:4">
       <c r="B39" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
         <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>165</v>
+        <v>371</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -3614,16 +3705,16 @@
     </row>
     <row r="40" spans="4:4">
       <c r="B40" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="F40" t="s">
         <v>58</v>
@@ -3631,7 +3722,7 @@
     </row>
     <row r="41" spans="4:4">
       <c r="B41" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="C41" t="s">
         <v>95</v>
@@ -3640,7 +3731,7 @@
         <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F41" t="s">
         <v>58</v>
@@ -3648,7 +3739,7 @@
     </row>
     <row r="42" spans="4:4">
       <c r="B42" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
         <v>95</v>
@@ -3657,7 +3748,7 @@
         <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="F42" t="s">
         <v>58</v>
@@ -3665,7 +3756,7 @@
     </row>
     <row r="43" spans="4:4">
       <c r="B43" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C43" t="s">
         <v>95</v>
@@ -3674,7 +3765,7 @@
         <v>61</v>
       </c>
       <c r="E43" t="s">
-        <v>372</v>
+        <v>209</v>
       </c>
       <c r="F43" t="s">
         <v>58</v>
@@ -3682,16 +3773,16 @@
     </row>
     <row r="44" spans="4:4">
       <c r="B44" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -3699,16 +3790,16 @@
     </row>
     <row r="45" spans="4:4">
       <c r="B45" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C45" t="s">
         <v>95</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
         <v>58</v>
@@ -3716,16 +3807,16 @@
     </row>
     <row r="46" spans="4:4">
       <c r="B46" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>92</v>
       </c>
       <c r="F46" t="s">
         <v>58</v>
@@ -3733,16 +3824,16 @@
     </row>
     <row r="47" spans="4:4">
       <c r="B47" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="F47" t="s">
         <v>58</v>
@@ -3750,16 +3841,16 @@
     </row>
     <row r="48" spans="4:4">
       <c r="B48" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="F48" t="s">
         <v>58</v>
@@ -3767,7 +3858,7 @@
     </row>
     <row r="49" spans="4:4">
       <c r="B49" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
@@ -3776,7 +3867,7 @@
         <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>222</v>
       </c>
       <c r="F49" t="s">
         <v>58</v>
@@ -3784,16 +3875,16 @@
     </row>
     <row r="50" spans="4:4">
       <c r="B50" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
       </c>
       <c r="E50" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="F50" t="s">
         <v>58</v>
@@ -3801,16 +3892,16 @@
     </row>
     <row r="51" spans="4:4">
       <c r="B51" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="F51" t="s">
         <v>58</v>
@@ -3818,16 +3909,16 @@
     </row>
     <row r="52" spans="4:4">
       <c r="B52" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E52" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F52" t="s">
         <v>58</v>
@@ -3835,16 +3926,16 @@
     </row>
     <row r="53" spans="4:4">
       <c r="B53" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E53" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F53" t="s">
         <v>58</v>
@@ -3852,16 +3943,16 @@
     </row>
     <row r="54" spans="4:4">
       <c r="B54" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
@@ -3869,16 +3960,16 @@
     </row>
     <row r="55" spans="4:4">
       <c r="B55" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C55" t="s">
         <v>95</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E55" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="F55" t="s">
         <v>58</v>
@@ -3886,16 +3977,16 @@
     </row>
     <row r="56" spans="4:4">
       <c r="B56" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
-        <v>226</v>
+        <v>99</v>
       </c>
       <c r="F56" t="s">
         <v>58</v>
@@ -3903,16 +3994,16 @@
     </row>
     <row r="57" spans="4:4">
       <c r="B57" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D57" t="s">
         <v>61</v>
       </c>
       <c r="E57" t="s">
-        <v>231</v>
+        <v>101</v>
       </c>
       <c r="F57" t="s">
         <v>58</v>
@@ -3920,7 +4011,7 @@
     </row>
     <row r="58" spans="4:4">
       <c r="B58" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C58" t="s">
         <v>96</v>
@@ -3937,7 +4028,7 @@
     </row>
     <row r="59" spans="4:4">
       <c r="B59" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C59" t="s">
         <v>96</v>
@@ -3954,16 +4045,16 @@
     </row>
     <row r="60" spans="4:4">
       <c r="B60" t="s">
-        <v>236</v>
+        <v>322</v>
       </c>
       <c r="C60" t="s">
         <v>96</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="F60" t="s">
         <v>58</v>
@@ -3971,16 +4062,16 @@
     </row>
     <row r="61" spans="4:4">
       <c r="B61" t="s">
-        <v>237</v>
+        <v>323</v>
       </c>
       <c r="C61" t="s">
         <v>96</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="F61" t="s">
         <v>58</v>
@@ -3988,7 +4079,7 @@
     </row>
     <row r="62" spans="4:4">
       <c r="B62" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C62" t="s">
         <v>96</v>
@@ -3997,7 +4088,7 @@
         <v>57</v>
       </c>
       <c r="E62" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F62" t="s">
         <v>58</v>
@@ -4005,7 +4096,7 @@
     </row>
     <row r="63" spans="4:4">
       <c r="B63" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C63" t="s">
         <v>96</v>
@@ -4014,7 +4105,7 @@
         <v>57</v>
       </c>
       <c r="E63" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F63" t="s">
         <v>58</v>
@@ -4022,7 +4113,7 @@
     </row>
     <row r="64" spans="4:4">
       <c r="B64" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C64" t="s">
         <v>96</v>
@@ -4031,7 +4122,7 @@
         <v>57</v>
       </c>
       <c r="E64" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F64" t="s">
         <v>58</v>
@@ -4039,7 +4130,7 @@
     </row>
     <row r="65" spans="4:4">
       <c r="B65" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C65" t="s">
         <v>96</v>
@@ -4048,7 +4139,7 @@
         <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F65" t="s">
         <v>58</v>
@@ -4056,7 +4147,7 @@
     </row>
     <row r="66" spans="4:4">
       <c r="B66" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C66" t="s">
         <v>96</v>
@@ -4065,7 +4156,7 @@
         <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F66" t="s">
         <v>58</v>
@@ -4073,7 +4164,7 @@
     </row>
     <row r="67" spans="4:4">
       <c r="B67" t="s">
-        <v>327</v>
+        <v>363</v>
       </c>
       <c r="C67" t="s">
         <v>96</v>
@@ -4082,7 +4173,7 @@
         <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F67" t="s">
         <v>58</v>
@@ -4090,7 +4181,7 @@
     </row>
     <row r="68" spans="4:4">
       <c r="B68" t="s">
-        <v>328</v>
+        <v>364</v>
       </c>
       <c r="C68" t="s">
         <v>96</v>
@@ -4099,7 +4190,7 @@
         <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F68" t="s">
         <v>58</v>
@@ -4107,16 +4198,16 @@
     </row>
     <row r="69" spans="4:4">
       <c r="B69" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
       <c r="C69" t="s">
         <v>96</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>342</v>
+        <v>194</v>
       </c>
       <c r="F69" t="s">
         <v>58</v>
@@ -4124,16 +4215,16 @@
     </row>
     <row r="70" spans="4:4">
       <c r="B70" t="s">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="C70" t="s">
         <v>96</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>344</v>
+        <v>196</v>
       </c>
       <c r="F70" t="s">
         <v>58</v>
@@ -4141,16 +4232,16 @@
     </row>
     <row r="71" spans="4:4">
       <c r="B71" t="s">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="C71" t="s">
         <v>96</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E71" t="s">
-        <v>346</v>
+        <v>198</v>
       </c>
       <c r="F71" t="s">
         <v>58</v>
@@ -4158,7 +4249,7 @@
     </row>
     <row r="72" spans="4:4">
       <c r="B72" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C72" t="s">
         <v>96</v>
@@ -4167,7 +4258,7 @@
         <v>57</v>
       </c>
       <c r="E72" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F72" t="s">
         <v>58</v>
@@ -4175,7 +4266,7 @@
     </row>
     <row r="73" spans="4:4">
       <c r="B73" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C73" t="s">
         <v>96</v>
@@ -4184,7 +4275,7 @@
         <v>57</v>
       </c>
       <c r="E73" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F73" t="s">
         <v>58</v>
@@ -4192,7 +4283,7 @@
     </row>
     <row r="74" spans="4:4">
       <c r="B74" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="C74" t="s">
         <v>96</v>
@@ -4201,7 +4292,7 @@
         <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>194</v>
+        <v>48</v>
       </c>
       <c r="F74" t="s">
         <v>58</v>
@@ -4209,16 +4300,16 @@
     </row>
     <row r="75" spans="4:4">
       <c r="B75" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
       </c>
       <c r="D75" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E75" t="s">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="F75" t="s">
         <v>58</v>
@@ -4226,16 +4317,16 @@
     </row>
     <row r="76" spans="4:4">
       <c r="B76" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
       <c r="C76" t="s">
         <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E76" t="s">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="F76" t="s">
         <v>58</v>
@@ -4243,16 +4334,16 @@
     </row>
     <row r="77" spans="4:4">
       <c r="B77" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="C77" t="s">
         <v>96</v>
       </c>
       <c r="D77" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E77" t="s">
-        <v>200</v>
+        <v>99</v>
       </c>
       <c r="F77" t="s">
         <v>58</v>
@@ -4260,16 +4351,16 @@
     </row>
     <row r="78" spans="4:4">
       <c r="B78" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="C78" t="s">
         <v>96</v>
       </c>
       <c r="D78" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E78" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="F78" t="s">
         <v>58</v>
@@ -4277,16 +4368,16 @@
     </row>
     <row r="79" spans="4:4">
       <c r="B79" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="C79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>48</v>
+        <v>390</v>
       </c>
       <c r="F79" t="s">
         <v>58</v>
@@ -4294,16 +4385,16 @@
     </row>
     <row r="80" spans="4:4">
       <c r="B80" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="C80" t="s">
         <v>42</v>
       </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E80" t="s">
-        <v>383</v>
+        <v>115</v>
       </c>
       <c r="F80" t="s">
         <v>58</v>
@@ -4311,16 +4402,16 @@
     </row>
     <row r="81" spans="4:4">
       <c r="B81" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D81" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E81" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="F81" t="s">
         <v>58</v>
@@ -4328,16 +4419,16 @@
     </row>
     <row r="82" spans="4:4">
       <c r="B82" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="C82" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E82" t="s">
-        <v>99</v>
+        <v>394</v>
       </c>
       <c r="F82" t="s">
         <v>58</v>
@@ -4345,16 +4436,16 @@
     </row>
     <row r="83" spans="4:4">
       <c r="B83" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C83" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D83" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E83" t="s">
-        <v>101</v>
+        <v>396</v>
       </c>
       <c r="F83" t="s">
         <v>58</v>
@@ -4362,16 +4453,16 @@
     </row>
     <row r="84" spans="4:4">
       <c r="B84" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="C84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D84" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E84" t="s">
-        <v>99</v>
+        <v>398</v>
       </c>
       <c r="F84" t="s">
         <v>58</v>
@@ -4379,16 +4470,16 @@
     </row>
     <row r="85" spans="4:4">
       <c r="B85" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="C85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D85" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E85" t="s">
-        <v>101</v>
+        <v>390</v>
       </c>
       <c r="F85" t="s">
         <v>58</v>
@@ -4396,16 +4487,16 @@
     </row>
     <row r="86" spans="4:4">
       <c r="B86" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="C86" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D86" t="s">
         <v>57</v>
       </c>
       <c r="E86" t="s">
-        <v>390</v>
+        <v>115</v>
       </c>
       <c r="F86" t="s">
         <v>58</v>
@@ -4413,7 +4504,7 @@
     </row>
     <row r="87" spans="4:4">
       <c r="B87" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C87" t="s">
         <v>42</v>
@@ -4430,7 +4521,7 @@
     </row>
     <row r="88" spans="4:4">
       <c r="B88" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="C88" t="s">
         <v>42</v>
@@ -4439,7 +4530,7 @@
         <v>57</v>
       </c>
       <c r="E88" t="s">
-        <v>115</v>
+        <v>394</v>
       </c>
       <c r="F88" t="s">
         <v>58</v>
@@ -4447,7 +4538,7 @@
     </row>
     <row r="89" spans="4:4">
       <c r="B89" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="C89" t="s">
         <v>42</v>
@@ -4456,7 +4547,7 @@
         <v>57</v>
       </c>
       <c r="E89" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F89" t="s">
         <v>58</v>
@@ -4464,16 +4555,16 @@
     </row>
     <row r="90" spans="4:4">
       <c r="B90" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="C90" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D90" t="s">
         <v>57</v>
       </c>
       <c r="E90" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F90" t="s">
         <v>58</v>
@@ -4481,16 +4572,16 @@
     </row>
     <row r="91" spans="4:4">
       <c r="B91" t="s">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="C91" t="s">
-        <v>95</v>
+        <v>417</v>
       </c>
       <c r="D91" t="s">
         <v>57</v>
       </c>
       <c r="E91" t="s">
-        <v>398</v>
+        <v>115</v>
       </c>
       <c r="F91" t="s">
         <v>58</v>
@@ -4498,16 +4589,16 @@
     </row>
     <row r="92" spans="4:4">
       <c r="B92" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="C92" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D92" t="s">
         <v>57</v>
       </c>
       <c r="E92" t="s">
-        <v>390</v>
+        <v>421</v>
       </c>
       <c r="F92" t="s">
         <v>58</v>
@@ -4515,16 +4606,16 @@
     </row>
     <row r="93" spans="4:4">
       <c r="B93" t="s">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="C93" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D93" t="s">
         <v>57</v>
       </c>
       <c r="E93" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="F93" t="s">
         <v>58</v>
@@ -4532,7 +4623,7 @@
     </row>
     <row r="94" spans="4:4">
       <c r="B94" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="C94" t="s">
         <v>42</v>
@@ -4549,7 +4640,7 @@
     </row>
     <row r="95" spans="4:4">
       <c r="B95" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="C95" t="s">
         <v>42</v>
@@ -4558,7 +4649,7 @@
         <v>57</v>
       </c>
       <c r="E95" t="s">
-        <v>394</v>
+        <v>115</v>
       </c>
       <c r="F95" t="s">
         <v>58</v>
@@ -4566,16 +4657,16 @@
     </row>
     <row r="96" spans="4:4">
       <c r="B96" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="C96" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D96" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E96" t="s">
-        <v>396</v>
+        <v>342</v>
       </c>
       <c r="F96" t="s">
         <v>58</v>
@@ -4583,16 +4674,16 @@
     </row>
     <row r="97" spans="4:4">
       <c r="B97" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
       <c r="C97" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E97" t="s">
-        <v>398</v>
+        <v>344</v>
       </c>
       <c r="F97" t="s">
         <v>58</v>
@@ -4600,16 +4691,16 @@
     </row>
     <row r="98" spans="4:4">
       <c r="B98" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D98" t="s">
         <v>61</v>
       </c>
       <c r="E98" t="s">
-        <v>209</v>
+        <v>346</v>
       </c>
       <c r="F98" t="s">
         <v>58</v>
@@ -4617,16 +4708,16 @@
     </row>
     <row r="99" spans="4:4">
       <c r="B99" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="C99" t="s">
-        <v>42</v>
+        <v>417</v>
       </c>
       <c r="D99" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E99" t="s">
-        <v>419</v>
+        <v>383</v>
       </c>
       <c r="F99" t="s">
         <v>58</v>
@@ -4634,16 +4725,16 @@
     </row>
     <row r="100" spans="4:4">
       <c r="B100" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="C100" t="s">
         <v>95</v>
       </c>
       <c r="D100" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E100" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="F100" t="s">
         <v>58</v>
@@ -4651,7 +4742,7 @@
     </row>
     <row r="101" spans="4:4">
       <c r="B101" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
       <c r="C101" t="s">
         <v>95</v>
@@ -4660,7 +4751,7 @@
         <v>61</v>
       </c>
       <c r="E101" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="F101" t="s">
         <v>58</v>
@@ -4668,16 +4759,16 @@
     </row>
     <row r="102" spans="4:4">
       <c r="B102" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="C102" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D102" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E102" t="s">
-        <v>92</v>
+        <v>380</v>
       </c>
       <c r="F102" t="s">
         <v>58</v>
@@ -4685,16 +4776,16 @@
     </row>
     <row r="103" spans="4:4">
       <c r="B103" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="C103" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D103" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E103" t="s">
-        <v>381</v>
+        <v>90</v>
       </c>
       <c r="F103" t="s">
         <v>58</v>
@@ -4702,16 +4793,16 @@
     </row>
     <row r="104" spans="4:4">
       <c r="B104" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="C104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D104" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E104" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="F104" t="s">
         <v>58</v>
@@ -4719,16 +4810,16 @@
     </row>
     <row r="105" spans="4:4">
       <c r="B105" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="C105" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D105" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E105" t="s">
-        <v>419</v>
+        <v>92</v>
       </c>
       <c r="F105" t="s">
         <v>58</v>
@@ -4736,16 +4827,16 @@
     </row>
     <row r="106" spans="4:4">
       <c r="B106" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="C106" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D106" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E106" t="s">
-        <v>224</v>
+        <v>381</v>
       </c>
       <c r="F106" t="s">
         <v>58</v>
@@ -4753,16 +4844,16 @@
     </row>
     <row r="107" spans="4:4">
       <c r="B107" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="C107" t="s">
         <v>96</v>
       </c>
       <c r="D107" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E107" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="F107" t="s">
         <v>58</v>
@@ -4770,7 +4861,7 @@
     </row>
     <row r="108" spans="4:4">
       <c r="B108" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="C108" t="s">
         <v>42</v>
@@ -4779,7 +4870,7 @@
         <v>68</v>
       </c>
       <c r="E108" t="s">
-        <v>419</v>
+        <v>439</v>
       </c>
       <c r="F108" t="s">
         <v>58</v>
@@ -4787,7 +4878,7 @@
     </row>
     <row r="109" spans="4:4">
       <c r="B109" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="C109" t="s">
         <v>95</v>
@@ -4804,7 +4895,7 @@
     </row>
     <row r="110" spans="4:4">
       <c r="B110" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="C110" t="s">
         <v>96</v>
@@ -4813,7 +4904,7 @@
         <v>61</v>
       </c>
       <c r="E110" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F110" t="s">
         <v>58</v>
@@ -4821,16 +4912,16 @@
     </row>
     <row r="111" spans="4:4">
       <c r="B111" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C111" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D111" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E111" t="s">
-        <v>190</v>
+        <v>439</v>
       </c>
       <c r="F111" t="s">
         <v>58</v>
@@ -4838,16 +4929,16 @@
     </row>
     <row r="112" spans="4:4">
       <c r="B112" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="C112" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D112" t="s">
         <v>57</v>
       </c>
       <c r="E112" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="F112" t="s">
         <v>58</v>
@@ -4855,16 +4946,16 @@
     </row>
     <row r="113" spans="4:4">
       <c r="B113" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="C113" t="s">
         <v>96</v>
       </c>
       <c r="D113" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E113" t="s">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="F113" t="s">
         <v>58</v>
@@ -4872,7 +4963,7 @@
     </row>
     <row r="114" spans="4:4">
       <c r="B114" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="C114" t="s">
         <v>96</v>
@@ -4881,7 +4972,7 @@
         <v>57</v>
       </c>
       <c r="E114" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F114" t="s">
         <v>58</v>
@@ -4889,7 +4980,7 @@
     </row>
     <row r="115" spans="4:4">
       <c r="B115" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="C115" t="s">
         <v>96</v>
@@ -4898,7 +4989,7 @@
         <v>57</v>
       </c>
       <c r="E115" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F115" t="s">
         <v>58</v>
@@ -4906,7 +4997,7 @@
     </row>
     <row r="116" spans="4:4">
       <c r="B116" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="C116" t="s">
         <v>96</v>
@@ -4915,7 +5006,7 @@
         <v>57</v>
       </c>
       <c r="E116" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F116" t="s">
         <v>58</v>
@@ -4923,7 +5014,7 @@
     </row>
     <row r="117" spans="4:4">
       <c r="B117" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="C117" t="s">
         <v>96</v>
@@ -4932,7 +5023,7 @@
         <v>57</v>
       </c>
       <c r="E117" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F117" t="s">
         <v>58</v>
@@ -4940,16 +5031,16 @@
     </row>
     <row r="118" spans="4:4">
       <c r="B118" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="C118" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D118" t="s">
         <v>57</v>
       </c>
       <c r="E118" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="F118" t="s">
         <v>58</v>
@@ -4957,16 +5048,16 @@
     </row>
     <row r="119" spans="4:4">
       <c r="B119" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="C119" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D119" t="s">
         <v>57</v>
       </c>
       <c r="E119" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="F119" t="s">
         <v>58</v>
@@ -4974,16 +5065,16 @@
     </row>
     <row r="120" spans="4:4">
       <c r="B120" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D120" t="s">
         <v>57</v>
       </c>
       <c r="E120" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
       <c r="F120" t="s">
         <v>58</v>
@@ -4991,7 +5082,7 @@
     </row>
     <row r="121" spans="4:4">
       <c r="B121" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="C121" t="s">
         <v>42</v>
@@ -5000,7 +5091,7 @@
         <v>57</v>
       </c>
       <c r="E121" t="s">
-        <v>83</v>
+        <v>160</v>
       </c>
       <c r="F121" t="s">
         <v>58</v>
@@ -5008,7 +5099,7 @@
     </row>
     <row r="122" spans="4:4">
       <c r="B122" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="C122" t="s">
         <v>95</v>
@@ -5017,7 +5108,7 @@
         <v>57</v>
       </c>
       <c r="E122" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="F122" t="s">
         <v>58</v>
@@ -5025,16 +5116,16 @@
     </row>
     <row r="123" spans="4:4">
       <c r="B123" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="C123" t="s">
         <v>95</v>
       </c>
       <c r="D123" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E123" t="s">
-        <v>46</v>
+        <v>455</v>
       </c>
       <c r="F123" t="s">
         <v>58</v>
@@ -5042,7 +5133,7 @@
     </row>
     <row r="124" spans="4:4">
       <c r="B124" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="C124" t="s">
         <v>95</v>
@@ -5051,7 +5142,7 @@
         <v>57</v>
       </c>
       <c r="E124" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F124" t="s">
         <v>58</v>
@@ -5059,25 +5150,89 @@
     </row>
     <row r="125" spans="4:4">
       <c r="B125" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="C125" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D125" t="s">
         <v>57</v>
       </c>
       <c r="E125" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F125" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="4:4"/>
-    <row r="127" spans="4:4"/>
-    <row r="128" spans="4:4"/>
-    <row r="129" spans="4:4"/>
+    <row r="126" spans="4:4">
+      <c r="B126" t="s">
+        <v>459</v>
+      </c>
+      <c r="C126" t="s">
+        <v>96</v>
+      </c>
+      <c r="D126" t="s">
+        <v>57</v>
+      </c>
+      <c r="E126" t="s">
+        <v>48</v>
+      </c>
+      <c r="F126" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4">
+      <c r="B127" t="s">
+        <v>460</v>
+      </c>
+      <c r="C127" t="s">
+        <v>96</v>
+      </c>
+      <c r="D127" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" t="s">
+        <v>48</v>
+      </c>
+      <c r="F127" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4">
+      <c r="B128" t="s">
+        <v>461</v>
+      </c>
+      <c r="C128" t="s">
+        <v>96</v>
+      </c>
+      <c r="D128" t="s">
+        <v>57</v>
+      </c>
+      <c r="E128" t="s">
+        <v>48</v>
+      </c>
+      <c r="F128" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4">
+      <c r="B129" t="s">
+        <v>462</v>
+      </c>
+      <c r="C129" t="s">
+        <v>96</v>
+      </c>
+      <c r="D129" t="s">
+        <v>57</v>
+      </c>
+      <c r="E129" t="s">
+        <v>48</v>
+      </c>
+      <c r="F129" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="130" spans="4:4"/>
     <row r="131" spans="4:4"/>
     <row r="132" spans="4:4"/>

</xml_diff>

<commit_message>
fixed bugs in automatical work mode
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37484" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76617" uniqueCount="554">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1534,6 +1534,361 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">остоновить расписание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Запущен режим расписания
+сушка будет запущена 
+автоматически 
+в назначеное время </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Запущен режим расписания
+сушка будет запущена 
+автоматически 
+в назначеное время </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Запущен режим расписания
+сушка будет запущена 
+автоматически 
+в назначеное время </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Запущен режим расписания
+сушка будет запущена 
+автоматически 
+в назначеное время </t>
+  </si>
+  <si>
+    <t xml:space="preserve">старт:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет связи с контроллером</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требуется сервисное обслуживание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">старт:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;ч.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;м.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t=&lt;value&gt;C°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">одежда:&lt;value&gt;ч.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">обувь:&lt;value&gt;ч.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">одежда:&lt;value&gt;м.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">обувь:&lt;value&gt;м.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие,
+не более 10 заданий на сутки,
+ либо на это время уже запланирована сушка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">textbt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЗАПУСТИТЬ РАСПИСАНИЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОСТОНОВИТЬ РАСПИСАНИЕ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пн</t>
+  </si>
+  <si>
+    <t xml:space="preserve">вт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ср</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x000-0xFFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет связи с контроллером!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требуется сервисное обслуживание!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Список событий пуст!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже запланировано, 
+или количество событий достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нельзя добавить новое событие!
+Возможно событие на это время уже
+запланировано,  или количество событий
+достигло десяти.</t>
   </si>
 </sst>
 </file>
@@ -2878,7 +3233,7 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>457</v>
+        <v>536</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2916,7 +3271,7 @@
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>457</v>
+        <v>536</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -2990,7 +3345,7 @@
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>457</v>
+        <v>536</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -3009,6 +3364,25 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>527</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:15">
@@ -3153,7 +3527,7 @@
         <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>466</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
@@ -3289,7 +3663,7 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>466</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -3589,7 +3963,7 @@
         <v>173</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>527</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -3657,7 +4031,7 @@
         <v>157</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>527</v>
       </c>
       <c r="D37" t="s">
         <v>61</v>
@@ -3691,13 +4065,13 @@
         <v>186</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>527</v>
       </c>
       <c r="D39" t="s">
         <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>371</v>
+        <v>528</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -3708,7 +4082,7 @@
         <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>527</v>
       </c>
       <c r="D40" t="s">
         <v>61</v>
@@ -3725,7 +4099,7 @@
         <v>203</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>527</v>
       </c>
       <c r="D41" t="s">
         <v>61</v>
@@ -3742,7 +4116,7 @@
         <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>527</v>
       </c>
       <c r="D42" t="s">
         <v>61</v>
@@ -4292,7 +4666,7 @@
         <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>48</v>
+        <v>503</v>
       </c>
       <c r="F74" t="s">
         <v>58</v>
@@ -4657,16 +5031,16 @@
     </row>
     <row r="96" spans="4:4">
       <c r="B96" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>417</v>
       </c>
       <c r="D96" t="s">
         <v>61</v>
       </c>
       <c r="E96" t="s">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="F96" t="s">
         <v>58</v>
@@ -4674,16 +5048,16 @@
     </row>
     <row r="97" spans="4:4">
       <c r="B97" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D97" t="s">
         <v>61</v>
       </c>
       <c r="E97" t="s">
-        <v>344</v>
+        <v>181</v>
       </c>
       <c r="F97" t="s">
         <v>58</v>
@@ -4691,16 +5065,16 @@
     </row>
     <row r="98" spans="4:4">
       <c r="B98" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>527</v>
       </c>
       <c r="D98" t="s">
         <v>61</v>
       </c>
       <c r="E98" t="s">
-        <v>346</v>
+        <v>209</v>
       </c>
       <c r="F98" t="s">
         <v>58</v>
@@ -4708,16 +5082,16 @@
     </row>
     <row r="99" spans="4:4">
       <c r="B99" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C99" t="s">
-        <v>417</v>
+        <v>42</v>
       </c>
       <c r="D99" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F99" t="s">
         <v>58</v>
@@ -4725,16 +5099,16 @@
     </row>
     <row r="100" spans="4:4">
       <c r="B100" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C100" t="s">
         <v>95</v>
       </c>
       <c r="D100" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E100" t="s">
-        <v>181</v>
+        <v>90</v>
       </c>
       <c r="F100" t="s">
         <v>58</v>
@@ -4742,16 +5116,16 @@
     </row>
     <row r="101" spans="4:4">
       <c r="B101" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>527</v>
       </c>
       <c r="D101" t="s">
         <v>61</v>
       </c>
       <c r="E101" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="F101" t="s">
         <v>58</v>
@@ -4759,16 +5133,16 @@
     </row>
     <row r="102" spans="4:4">
       <c r="B102" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C102" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D102" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E102" t="s">
-        <v>380</v>
+        <v>92</v>
       </c>
       <c r="F102" t="s">
         <v>58</v>
@@ -4776,16 +5150,16 @@
     </row>
     <row r="103" spans="4:4">
       <c r="B103" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C103" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D103" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E103" t="s">
-        <v>90</v>
+        <v>381</v>
       </c>
       <c r="F103" t="s">
         <v>58</v>
@@ -4793,16 +5167,16 @@
     </row>
     <row r="104" spans="4:4">
       <c r="B104" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C104" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D104" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E104" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F104" t="s">
         <v>58</v>
@@ -4810,16 +5184,16 @@
     </row>
     <row r="105" spans="4:4">
       <c r="B105" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C105" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D105" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E105" t="s">
-        <v>92</v>
+        <v>439</v>
       </c>
       <c r="F105" t="s">
         <v>58</v>
@@ -4827,16 +5201,16 @@
     </row>
     <row r="106" spans="4:4">
       <c r="B106" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C106" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D106" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E106" t="s">
-        <v>381</v>
+        <v>224</v>
       </c>
       <c r="F106" t="s">
         <v>58</v>
@@ -4844,16 +5218,16 @@
     </row>
     <row r="107" spans="4:4">
       <c r="B107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C107" t="s">
         <v>96</v>
       </c>
       <c r="D107" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E107" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="F107" t="s">
         <v>58</v>
@@ -4861,7 +5235,7 @@
     </row>
     <row r="108" spans="4:4">
       <c r="B108" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C108" t="s">
         <v>42</v>
@@ -4878,7 +5252,7 @@
     </row>
     <row r="109" spans="4:4">
       <c r="B109" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C109" t="s">
         <v>95</v>
@@ -4895,7 +5269,7 @@
     </row>
     <row r="110" spans="4:4">
       <c r="B110" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C110" t="s">
         <v>96</v>
@@ -4904,7 +5278,7 @@
         <v>61</v>
       </c>
       <c r="E110" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F110" t="s">
         <v>58</v>
@@ -4912,16 +5286,16 @@
     </row>
     <row r="111" spans="4:4">
       <c r="B111" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C111" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D111" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E111" t="s">
-        <v>439</v>
+        <v>190</v>
       </c>
       <c r="F111" t="s">
         <v>58</v>
@@ -4929,16 +5303,16 @@
     </row>
     <row r="112" spans="4:4">
       <c r="B112" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C112" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D112" t="s">
         <v>57</v>
       </c>
       <c r="E112" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="F112" t="s">
         <v>58</v>
@@ -4946,16 +5320,16 @@
     </row>
     <row r="113" spans="4:4">
       <c r="B113" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C113" t="s">
         <v>96</v>
       </c>
       <c r="D113" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E113" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="F113" t="s">
         <v>58</v>
@@ -4963,7 +5337,7 @@
     </row>
     <row r="114" spans="4:4">
       <c r="B114" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C114" t="s">
         <v>96</v>
@@ -4972,7 +5346,7 @@
         <v>57</v>
       </c>
       <c r="E114" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F114" t="s">
         <v>58</v>
@@ -4980,7 +5354,7 @@
     </row>
     <row r="115" spans="4:4">
       <c r="B115" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C115" t="s">
         <v>96</v>
@@ -4989,7 +5363,7 @@
         <v>57</v>
       </c>
       <c r="E115" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="F115" t="s">
         <v>58</v>
@@ -4997,7 +5371,7 @@
     </row>
     <row r="116" spans="4:4">
       <c r="B116" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C116" t="s">
         <v>96</v>
@@ -5006,7 +5380,7 @@
         <v>57</v>
       </c>
       <c r="E116" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F116" t="s">
         <v>58</v>
@@ -5014,7 +5388,7 @@
     </row>
     <row r="117" spans="4:4">
       <c r="B117" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C117" t="s">
         <v>96</v>
@@ -5023,7 +5397,7 @@
         <v>57</v>
       </c>
       <c r="E117" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F117" t="s">
         <v>58</v>
@@ -5031,16 +5405,16 @@
     </row>
     <row r="118" spans="4:4">
       <c r="B118" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C118" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D118" t="s">
         <v>57</v>
       </c>
       <c r="E118" t="s">
-        <v>198</v>
+        <v>466</v>
       </c>
       <c r="F118" t="s">
         <v>58</v>
@@ -5048,16 +5422,16 @@
     </row>
     <row r="119" spans="4:4">
       <c r="B119" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D119" t="s">
         <v>57</v>
       </c>
       <c r="E119" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="F119" t="s">
         <v>58</v>
@@ -5065,16 +5439,16 @@
     </row>
     <row r="120" spans="4:4">
       <c r="B120" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C120" t="s">
-        <v>96</v>
+        <v>527</v>
       </c>
       <c r="D120" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E120" t="s">
-        <v>202</v>
+        <v>455</v>
       </c>
       <c r="F120" t="s">
         <v>58</v>
@@ -5082,16 +5456,16 @@
     </row>
     <row r="121" spans="4:4">
       <c r="B121" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C121" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D121" t="s">
         <v>57</v>
       </c>
       <c r="E121" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="F121" t="s">
         <v>58</v>
@@ -5099,16 +5473,16 @@
     </row>
     <row r="122" spans="4:4">
       <c r="B122" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="C122" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D122" t="s">
         <v>57</v>
       </c>
       <c r="E122" t="s">
-        <v>88</v>
+        <v>508</v>
       </c>
       <c r="F122" t="s">
         <v>58</v>
@@ -5116,16 +5490,16 @@
     </row>
     <row r="123" spans="4:4">
       <c r="B123" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C123" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D123" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E123" t="s">
-        <v>455</v>
+        <v>509</v>
       </c>
       <c r="F123" t="s">
         <v>58</v>
@@ -5133,16 +5507,16 @@
     </row>
     <row r="124" spans="4:4">
       <c r="B124" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C124" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D124" t="s">
         <v>57</v>
       </c>
       <c r="E124" t="s">
-        <v>48</v>
+        <v>510</v>
       </c>
       <c r="F124" t="s">
         <v>58</v>
@@ -5150,7 +5524,7 @@
     </row>
     <row r="125" spans="4:4">
       <c r="B125" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C125" t="s">
         <v>96</v>
@@ -5159,7 +5533,7 @@
         <v>57</v>
       </c>
       <c r="E125" t="s">
-        <v>48</v>
+        <v>511</v>
       </c>
       <c r="F125" t="s">
         <v>58</v>
@@ -5167,7 +5541,7 @@
     </row>
     <row r="126" spans="4:4">
       <c r="B126" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C126" t="s">
         <v>96</v>
@@ -5176,7 +5550,7 @@
         <v>57</v>
       </c>
       <c r="E126" t="s">
-        <v>48</v>
+        <v>512</v>
       </c>
       <c r="F126" t="s">
         <v>58</v>
@@ -5184,16 +5558,16 @@
     </row>
     <row r="127" spans="4:4">
       <c r="B127" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C127" t="s">
         <v>96</v>
       </c>
       <c r="D127" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E127" t="s">
-        <v>48</v>
+        <v>342</v>
       </c>
       <c r="F127" t="s">
         <v>58</v>
@@ -5201,16 +5575,16 @@
     </row>
     <row r="128" spans="4:4">
       <c r="B128" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C128" t="s">
         <v>96</v>
       </c>
       <c r="D128" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E128" t="s">
-        <v>48</v>
+        <v>344</v>
       </c>
       <c r="F128" t="s">
         <v>58</v>
@@ -5218,46 +5592,446 @@
     </row>
     <row r="129" spans="4:4">
       <c r="B129" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C129" t="s">
         <v>96</v>
       </c>
       <c r="D129" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E129" t="s">
+        <v>346</v>
+      </c>
+      <c r="F129" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4">
+      <c r="B130" t="s">
+        <v>467</v>
+      </c>
+      <c r="C130" t="s">
+        <v>527</v>
+      </c>
+      <c r="D130" t="s">
+        <v>61</v>
+      </c>
+      <c r="E130" t="s">
+        <v>529</v>
+      </c>
+      <c r="F130" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4">
+      <c r="B131" t="s">
+        <v>469</v>
+      </c>
+      <c r="C131" t="s">
+        <v>96</v>
+      </c>
+      <c r="D131" t="s">
+        <v>61</v>
+      </c>
+      <c r="E131" t="s">
+        <v>470</v>
+      </c>
+      <c r="F131" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4">
+      <c r="B132" t="s">
+        <v>471</v>
+      </c>
+      <c r="C132" t="s">
+        <v>96</v>
+      </c>
+      <c r="D132" t="s">
+        <v>61</v>
+      </c>
+      <c r="E132" t="s">
+        <v>470</v>
+      </c>
+      <c r="F132" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4">
+      <c r="B133" t="s">
+        <v>476</v>
+      </c>
+      <c r="C133" t="s">
+        <v>40</v>
+      </c>
+      <c r="D133" t="s">
+        <v>57</v>
+      </c>
+      <c r="E133" t="s">
         <v>48</v>
       </c>
-      <c r="F129" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="130" spans="4:4"/>
-    <row r="131" spans="4:4"/>
-    <row r="132" spans="4:4"/>
-    <row r="133" spans="4:4"/>
-    <row r="134" spans="4:4"/>
-    <row r="135" spans="4:4"/>
-    <row r="136" spans="4:4"/>
-    <row r="137" spans="4:4"/>
-    <row r="138" spans="4:4"/>
-    <row r="139" spans="4:4"/>
-    <row r="140" spans="4:4"/>
-    <row r="141" spans="4:4"/>
-    <row r="142" spans="4:4"/>
-    <row r="143" spans="4:4"/>
-    <row r="144" spans="4:4"/>
-    <row r="145" spans="4:4"/>
-    <row r="146" spans="4:4"/>
-    <row r="147" spans="4:4"/>
-    <row r="148" spans="4:4"/>
-    <row r="149" spans="4:4"/>
-    <row r="150" spans="4:4"/>
-    <row r="151" spans="4:4"/>
-    <row r="152" spans="4:4"/>
-    <row r="153" spans="4:4"/>
-    <row r="154" spans="4:4"/>
+      <c r="F133" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4">
+      <c r="B134" t="s">
+        <v>477</v>
+      </c>
+      <c r="C134" t="s">
+        <v>40</v>
+      </c>
+      <c r="D134" t="s">
+        <v>57</v>
+      </c>
+      <c r="E134" t="s">
+        <v>530</v>
+      </c>
+      <c r="F134" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4">
+      <c r="B135" t="s">
+        <v>478</v>
+      </c>
+      <c r="C135" t="s">
+        <v>40</v>
+      </c>
+      <c r="D135" t="s">
+        <v>57</v>
+      </c>
+      <c r="E135" t="s">
+        <v>48</v>
+      </c>
+      <c r="F135" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4">
+      <c r="B136" t="s">
+        <v>479</v>
+      </c>
+      <c r="C136" t="s">
+        <v>40</v>
+      </c>
+      <c r="D136" t="s">
+        <v>57</v>
+      </c>
+      <c r="E136" t="s">
+        <v>531</v>
+      </c>
+      <c r="F136" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4">
+      <c r="B137" t="s">
+        <v>480</v>
+      </c>
+      <c r="C137" t="s">
+        <v>40</v>
+      </c>
+      <c r="D137" t="s">
+        <v>57</v>
+      </c>
+      <c r="E137" t="s">
+        <v>48</v>
+      </c>
+      <c r="F137" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4">
+      <c r="B138" t="s">
+        <v>481</v>
+      </c>
+      <c r="C138" t="s">
+        <v>40</v>
+      </c>
+      <c r="D138" t="s">
+        <v>57</v>
+      </c>
+      <c r="E138" t="s">
+        <v>532</v>
+      </c>
+      <c r="F138" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4">
+      <c r="B139" t="s">
+        <v>483</v>
+      </c>
+      <c r="C139" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139" t="s">
+        <v>57</v>
+      </c>
+      <c r="E139" t="s">
+        <v>48</v>
+      </c>
+      <c r="F139" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4">
+      <c r="B140" t="s">
+        <v>484</v>
+      </c>
+      <c r="C140" t="s">
+        <v>40</v>
+      </c>
+      <c r="D140" t="s">
+        <v>57</v>
+      </c>
+      <c r="E140" t="s">
+        <v>533</v>
+      </c>
+      <c r="F140" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4">
+      <c r="B141" t="s">
+        <v>485</v>
+      </c>
+      <c r="C141" t="s">
+        <v>40</v>
+      </c>
+      <c r="D141" t="s">
+        <v>57</v>
+      </c>
+      <c r="E141" t="s">
+        <v>48</v>
+      </c>
+      <c r="F141" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4">
+      <c r="B142" t="s">
+        <v>486</v>
+      </c>
+      <c r="C142" t="s">
+        <v>40</v>
+      </c>
+      <c r="D142" t="s">
+        <v>57</v>
+      </c>
+      <c r="E142" t="s">
+        <v>534</v>
+      </c>
+      <c r="F142" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4">
+      <c r="B143" t="s">
+        <v>487</v>
+      </c>
+      <c r="C143" t="s">
+        <v>40</v>
+      </c>
+      <c r="D143" t="s">
+        <v>57</v>
+      </c>
+      <c r="E143" t="s">
+        <v>48</v>
+      </c>
+      <c r="F143" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4">
+      <c r="B144" t="s">
+        <v>488</v>
+      </c>
+      <c r="C144" t="s">
+        <v>40</v>
+      </c>
+      <c r="D144" t="s">
+        <v>57</v>
+      </c>
+      <c r="E144" t="s">
+        <v>535</v>
+      </c>
+      <c r="F144" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4">
+      <c r="B145" t="s">
+        <v>489</v>
+      </c>
+      <c r="C145" t="s">
+        <v>40</v>
+      </c>
+      <c r="D145" t="s">
+        <v>57</v>
+      </c>
+      <c r="E145" t="s">
+        <v>48</v>
+      </c>
+      <c r="F145" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4">
+      <c r="B146" t="s">
+        <v>490</v>
+      </c>
+      <c r="C146" t="s">
+        <v>40</v>
+      </c>
+      <c r="D146" t="s">
+        <v>57</v>
+      </c>
+      <c r="E146" t="s">
+        <v>423</v>
+      </c>
+      <c r="F146" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4">
+      <c r="B147" t="s">
+        <v>491</v>
+      </c>
+      <c r="C147" t="s">
+        <v>96</v>
+      </c>
+      <c r="D147" t="s">
+        <v>57</v>
+      </c>
+      <c r="E147" t="s">
+        <v>48</v>
+      </c>
+      <c r="F147" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4">
+      <c r="B148" t="s">
+        <v>492</v>
+      </c>
+      <c r="C148" t="s">
+        <v>96</v>
+      </c>
+      <c r="D148" t="s">
+        <v>57</v>
+      </c>
+      <c r="E148" t="s">
+        <v>553</v>
+      </c>
+      <c r="F148" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4">
+      <c r="B149" t="s">
+        <v>494</v>
+      </c>
+      <c r="C149" t="s">
+        <v>85</v>
+      </c>
+      <c r="D149" t="s">
+        <v>61</v>
+      </c>
+      <c r="E149" t="s">
+        <v>48</v>
+      </c>
+      <c r="F149" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4">
+      <c r="B150" t="s">
+        <v>495</v>
+      </c>
+      <c r="C150" t="s">
+        <v>85</v>
+      </c>
+      <c r="D150" t="s">
+        <v>57</v>
+      </c>
+      <c r="E150" t="s">
+        <v>537</v>
+      </c>
+      <c r="F150" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4">
+      <c r="B151" t="s">
+        <v>497</v>
+      </c>
+      <c r="C151" t="s">
+        <v>85</v>
+      </c>
+      <c r="D151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E151" t="s">
+        <v>48</v>
+      </c>
+      <c r="F151" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4">
+      <c r="B152" t="s">
+        <v>498</v>
+      </c>
+      <c r="C152" t="s">
+        <v>85</v>
+      </c>
+      <c r="D152" t="s">
+        <v>57</v>
+      </c>
+      <c r="E152" t="s">
+        <v>538</v>
+      </c>
+      <c r="F152" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4">
+      <c r="B153" t="s">
+        <v>539</v>
+      </c>
+      <c r="C153" t="s">
+        <v>40</v>
+      </c>
+      <c r="D153" t="s">
+        <v>57</v>
+      </c>
+      <c r="E153" t="s">
+        <v>48</v>
+      </c>
+      <c r="F153" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4">
+      <c r="B154" t="s">
+        <v>540</v>
+      </c>
+      <c r="C154" t="s">
+        <v>40</v>
+      </c>
+      <c r="D154" t="s">
+        <v>57</v>
+      </c>
+      <c r="E154" t="s">
+        <v>541</v>
+      </c>
+      <c r="F154" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="155" spans="4:4"/>
     <row r="156" spans="4:4"/>
     <row r="157" spans="4:4"/>

</xml_diff>